<commit_message>
Updated data and OUT files with 2 corrected scale book numbers for Conuma 2022
</commit_message>
<xml_diff>
--- a/CON Fecundity Study 2022/ConumaChinookFecundityData_2022.xlsx
+++ b/CON Fecundity Study 2022/ConumaChinookFecundityData_2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brownn\Documents\WCVI\Chinook-fecundity\CON Fecundity Study 2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0987ADE6-1DBF-42F2-B234-7E4873E3B1C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8979D9BB-95E9-4600-8FF7-4881683B09B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0B77436E-E361-48C2-A30A-93B5611FB31F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="163">
   <si>
     <t xml:space="preserve"> =IF(N1="",((L1+M1)/20),((L1+M1+N1)/30))</t>
   </si>
@@ -539,6 +539,12 @@
   </si>
   <si>
     <t>% Diff betw subsamples 1 and 2</t>
+  </si>
+  <si>
+    <t>Changed scale book number from 17377 to 1036314 based on results from Age Batch File. Not sure why the difference. Nick Brown Nov 2023.</t>
+  </si>
+  <si>
+    <t>Changed scale book number from 17376 to 1036313 based on results from Age Batch File. Not sure why the difference. Nick Brown Nov 2023.</t>
   </si>
 </sst>
 </file>
@@ -2890,8 +2896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FE0EB01-1583-42A6-BDC3-9EA7A9E1F173}">
   <dimension ref="A1:AD126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+    <sheetView tabSelected="1" topLeftCell="D73" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H124" sqref="H124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11111,7 +11117,7 @@
         <v>805</v>
       </c>
       <c r="E104">
-        <v>17376</v>
+        <v>1036313</v>
       </c>
       <c r="F104">
         <v>1</v>
@@ -11171,7 +11177,9 @@
       <c r="AB104" s="29" t="s">
         <v>137</v>
       </c>
-      <c r="AC104" s="25"/>
+      <c r="AC104" s="25" t="s">
+        <v>162</v>
+      </c>
       <c r="AD104" s="64">
         <f t="shared" si="11"/>
         <v>2.109829804590465E-2</v>
@@ -11191,7 +11199,7 @@
         <v>800</v>
       </c>
       <c r="E105">
-        <v>17376</v>
+        <v>1036313</v>
       </c>
       <c r="F105">
         <v>2</v>
@@ -11251,7 +11259,9 @@
       <c r="AB105" s="29" t="s">
         <v>137</v>
       </c>
-      <c r="AC105" s="25"/>
+      <c r="AC105" s="25" t="s">
+        <v>162</v>
+      </c>
       <c r="AD105" s="64">
         <f t="shared" si="11"/>
         <v>4.4032968273682695E-3</v>
@@ -11271,7 +11281,7 @@
         <v>795</v>
       </c>
       <c r="E106">
-        <v>17376</v>
+        <v>1036313</v>
       </c>
       <c r="F106">
         <v>3</v>
@@ -11331,7 +11341,9 @@
       <c r="AB106" s="29" t="s">
         <v>137</v>
       </c>
-      <c r="AC106" s="25"/>
+      <c r="AC106" s="25" t="s">
+        <v>162</v>
+      </c>
       <c r="AD106" s="64">
         <f t="shared" si="11"/>
         <v>1.7754399636340006E-2</v>
@@ -11351,7 +11363,7 @@
         <v>800</v>
       </c>
       <c r="E107">
-        <v>17376</v>
+        <v>1036313</v>
       </c>
       <c r="F107">
         <v>4</v>
@@ -11411,7 +11423,9 @@
       <c r="AB107" s="29" t="s">
         <v>137</v>
       </c>
-      <c r="AC107" s="25"/>
+      <c r="AC107" s="25" t="s">
+        <v>162</v>
+      </c>
       <c r="AD107" s="64">
         <f t="shared" si="11"/>
         <v>2.3404474688112058E-2</v>
@@ -11431,7 +11445,7 @@
         <v>795</v>
       </c>
       <c r="E108">
-        <v>17376</v>
+        <v>1036313</v>
       </c>
       <c r="F108">
         <v>5</v>
@@ -11491,7 +11505,9 @@
       <c r="AB108" s="29" t="s">
         <v>137</v>
       </c>
-      <c r="AC108" s="25"/>
+      <c r="AC108" s="25" t="s">
+        <v>162</v>
+      </c>
       <c r="AD108" s="64">
         <f t="shared" si="11"/>
         <v>2.9222328244274268E-3</v>
@@ -11511,7 +11527,7 @@
         <v>580</v>
       </c>
       <c r="E109">
-        <v>17376</v>
+        <v>1036313</v>
       </c>
       <c r="F109">
         <v>6</v>
@@ -11571,7 +11587,9 @@
       <c r="AB109" s="29" t="s">
         <v>137</v>
       </c>
-      <c r="AC109" s="25"/>
+      <c r="AC109" s="25" t="s">
+        <v>162</v>
+      </c>
       <c r="AD109" s="64">
         <f t="shared" si="11"/>
         <v>1.8309186435280837E-2</v>
@@ -11590,8 +11608,8 @@
       <c r="D110" s="55">
         <v>560</v>
       </c>
-      <c r="E110" s="55">
-        <v>17376</v>
+      <c r="E110">
+        <v>1036313</v>
       </c>
       <c r="F110" s="55">
         <v>7</v>
@@ -11651,7 +11669,9 @@
       <c r="AB110" s="63" t="s">
         <v>137</v>
       </c>
-      <c r="AC110" s="56"/>
+      <c r="AC110" s="25" t="s">
+        <v>162</v>
+      </c>
       <c r="AD110" s="64">
         <f t="shared" si="11"/>
         <v>1.7891929151556893E-2</v>
@@ -11671,7 +11691,7 @@
         <v>795</v>
       </c>
       <c r="E111">
-        <v>17376</v>
+        <v>1036313</v>
       </c>
       <c r="F111">
         <v>8</v>
@@ -11731,7 +11751,9 @@
       <c r="AB111" s="29" t="s">
         <v>137</v>
       </c>
-      <c r="AC111" s="25"/>
+      <c r="AC111" s="25" t="s">
+        <v>162</v>
+      </c>
       <c r="AD111" s="64">
         <f t="shared" si="11"/>
         <v>5.2427184466019551E-2</v>
@@ -11751,7 +11773,7 @@
         <v>810</v>
       </c>
       <c r="E112">
-        <v>17376</v>
+        <v>1036313</v>
       </c>
       <c r="F112">
         <v>9</v>
@@ -11811,7 +11833,9 @@
       <c r="AB112" s="29" t="s">
         <v>137</v>
       </c>
-      <c r="AC112" s="25"/>
+      <c r="AC112" s="25" t="s">
+        <v>162</v>
+      </c>
       <c r="AD112" s="64">
         <f t="shared" si="11"/>
         <v>0.51302549194991065</v>
@@ -11831,7 +11855,7 @@
         <v>570</v>
       </c>
       <c r="E113">
-        <v>17376</v>
+        <v>1036313</v>
       </c>
       <c r="F113">
         <v>10</v>
@@ -11891,7 +11915,9 @@
       <c r="AB113" s="29" t="s">
         <v>137</v>
       </c>
-      <c r="AC113" s="25"/>
+      <c r="AC113" s="25" t="s">
+        <v>162</v>
+      </c>
       <c r="AD113" s="64">
         <f t="shared" si="11"/>
         <v>3.6961631716300472E-2</v>
@@ -11911,7 +11937,7 @@
         <v>795</v>
       </c>
       <c r="E114">
-        <v>17377</v>
+        <v>1036314</v>
       </c>
       <c r="F114">
         <v>1</v>
@@ -11971,7 +11997,9 @@
       <c r="AB114" s="29" t="s">
         <v>137</v>
       </c>
-      <c r="AC114" s="25"/>
+      <c r="AC114" s="25" t="s">
+        <v>161</v>
+      </c>
       <c r="AD114" s="64">
         <f t="shared" si="11"/>
         <v>8.1759557807459839E-3</v>
@@ -11991,7 +12019,7 @@
         <v>835</v>
       </c>
       <c r="E115">
-        <v>17377</v>
+        <v>1036314</v>
       </c>
       <c r="F115">
         <v>2</v>
@@ -12051,7 +12079,9 @@
       <c r="AB115" s="29" t="s">
         <v>137</v>
       </c>
-      <c r="AC115" s="25"/>
+      <c r="AC115" s="25" t="s">
+        <v>161</v>
+      </c>
       <c r="AD115" s="64">
         <f t="shared" si="11"/>
         <v>4.6685298025381489E-2</v>
@@ -12071,7 +12101,7 @@
         <v>585</v>
       </c>
       <c r="E116">
-        <v>17377</v>
+        <v>1036314</v>
       </c>
       <c r="F116">
         <v>3</v>
@@ -12131,7 +12161,9 @@
       <c r="AB116" s="29" t="s">
         <v>137</v>
       </c>
-      <c r="AC116" s="25"/>
+      <c r="AC116" s="25" t="s">
+        <v>161</v>
+      </c>
       <c r="AD116" s="64">
         <f t="shared" si="11"/>
         <v>3.453996983408749E-2</v>
@@ -12151,7 +12183,7 @@
         <v>795</v>
       </c>
       <c r="E117">
-        <v>17377</v>
+        <v>1036314</v>
       </c>
       <c r="F117">
         <v>4</v>
@@ -12211,7 +12243,9 @@
       <c r="AB117" s="29" t="s">
         <v>137</v>
       </c>
-      <c r="AC117" s="25"/>
+      <c r="AC117" s="25" t="s">
+        <v>161</v>
+      </c>
       <c r="AD117" s="64">
         <f t="shared" si="11"/>
         <v>1.6965232434845618E-2</v>
@@ -12231,7 +12265,7 @@
         <v>585</v>
       </c>
       <c r="E118">
-        <v>17377</v>
+        <v>1036314</v>
       </c>
       <c r="F118">
         <v>5</v>
@@ -12291,7 +12325,9 @@
       <c r="AB118" s="29" t="s">
         <v>137</v>
       </c>
-      <c r="AC118" s="25"/>
+      <c r="AC118" s="25" t="s">
+        <v>161</v>
+      </c>
       <c r="AD118" s="64">
         <f t="shared" si="11"/>
         <v>2.8238021487780499E-2</v>
@@ -12311,7 +12347,7 @@
         <v>586</v>
       </c>
       <c r="E119">
-        <v>17377</v>
+        <v>1036314</v>
       </c>
       <c r="F119">
         <v>6</v>
@@ -12371,7 +12407,9 @@
       <c r="AB119" s="29" t="s">
         <v>137</v>
       </c>
-      <c r="AC119" s="25"/>
+      <c r="AC119" s="25" t="s">
+        <v>161</v>
+      </c>
       <c r="AD119" s="64">
         <f t="shared" si="11"/>
         <v>0.13943501810455772</v>
@@ -12391,7 +12429,7 @@
         <v>805</v>
       </c>
       <c r="E120">
-        <v>17377</v>
+        <v>1036314</v>
       </c>
       <c r="F120">
         <v>7</v>
@@ -12451,7 +12489,9 @@
       <c r="AB120" s="29" t="s">
         <v>137</v>
       </c>
-      <c r="AC120" s="25"/>
+      <c r="AC120" s="25" t="s">
+        <v>161</v>
+      </c>
       <c r="AD120" s="64">
         <f t="shared" si="11"/>
         <v>1.1198678366374113E-2</v>
@@ -12471,7 +12511,7 @@
         <v>800</v>
       </c>
       <c r="E121">
-        <v>17377</v>
+        <v>1036314</v>
       </c>
       <c r="F121">
         <v>8</v>
@@ -12531,7 +12571,9 @@
       <c r="AB121" s="29" t="s">
         <v>137</v>
       </c>
-      <c r="AC121" s="25"/>
+      <c r="AC121" s="25" t="s">
+        <v>161</v>
+      </c>
       <c r="AD121" s="64">
         <f t="shared" si="11"/>
         <v>1.5180265654649036E-2</v>
@@ -12551,7 +12593,7 @@
         <v>565</v>
       </c>
       <c r="E122">
-        <v>17377</v>
+        <v>1036314</v>
       </c>
       <c r="F122">
         <v>9</v>
@@ -12611,7 +12653,9 @@
       <c r="AB122" s="29" t="s">
         <v>137</v>
       </c>
-      <c r="AC122" s="25"/>
+      <c r="AC122" s="25" t="s">
+        <v>161</v>
+      </c>
       <c r="AD122" s="64">
         <f t="shared" si="11"/>
         <v>4.6492873835620868E-2</v>
@@ -12631,7 +12675,7 @@
         <v>695</v>
       </c>
       <c r="E123">
-        <v>17377</v>
+        <v>1036314</v>
       </c>
       <c r="F123">
         <v>10</v>
@@ -12691,7 +12735,9 @@
       <c r="AB123" s="29" t="s">
         <v>137</v>
       </c>
-      <c r="AC123" s="25"/>
+      <c r="AC123" s="25" t="s">
+        <v>161</v>
+      </c>
       <c r="AD123" s="64">
         <f t="shared" si="11"/>
         <v>4.3587805492567334E-2</v>

</xml_diff>